<commit_message>
day 1 slides for 590 etc
</commit_message>
<xml_diff>
--- a/ids590_specific/class_schedule_590_xlsx.xlsx
+++ b/ids590_specific/class_schedule_590_xlsx.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids590_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB6ADF3-9AFB-DD4A-A3F0-85D4BA0CA3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B900696-2598-4B4A-9CEC-F9F8CE48C35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="500" windowWidth="35860" windowHeight="20940" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="2540" yWindow="500" windowWidth="35860" windowHeight="19720" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
-    <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
+    <sheet name="class_schedule_590" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="101">
   <si>
     <t>Topic</t>
   </si>
@@ -66,9 +66,6 @@
     <t>- Statistics with statsmodels</t>
   </si>
   <si>
-    <t>- Machine Learning with sckikit-learn</t>
-  </si>
-  <si>
     <t>- Pandas: Cleaning
 - Tracebacks</t>
   </si>
@@ -163,9 +160,6 @@
   </si>
   <si>
     <t>Thurs, Nov 21</t>
-  </si>
-  <si>
-    <t>**FALL BREAK** (Not technically, but take the week)</t>
   </si>
   <si>
     <t>LAST CLASS</t>
@@ -189,23 +183,6 @@
 - If you don't have a github account, make one. Register a passkey or at least two factor authentication.
 - `Add your ssh key to your github account &lt;https://docs.github.com/en/authentication/connecting-to-github-with-ssh/adding-a-new-ssh-key-to-your-github-account&gt;`_
 - `Visualize Git Branches &lt;https://learngitbranching.js.org/&gt;`_</t>
-  </si>
-  <si>
-    <t>- Under the numpy heading, `read everything under Vectors EXCEPT Speed/Ease of Use Tradeoff and Vectorization &lt;../notebooks/class_2/week_2/10_why_numpy.html&gt;`_
-- Under the numpy heading, also read everything under `Subsetting Vectors &lt;../notebooks/class_2/week_2/10_why_numpy.html&gt;`_
-- `Numbers in Computers &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/ints_and_floats.html&gt;`_
-- `Writing Good Notebooks &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/writing_good_jupyter_notebooks.html&gt;`_</t>
-  </si>
-  <si>
-    <t>**More Numpy Concepts:**
-- `Views and Copies &lt;../notebooks/class_2/week_3/10_views_and_copies.html&gt;`_
-- `When Do I Get a View &lt;../notebooks/class_2/week_3/11_when_do_I_get_a_view.html&gt;`_
-- `Variables, Objects, and Numpy &lt;../notebooks/class_2/week_3/13_objects_and_variables.html&gt;`_
-- `Views and Copies Recap &lt;../notebooks/class_2/week_3/12_views_and_copies_recap.html&gt;`_
-**Matrices:**
-- `Matrices — From Welcome through Review of Matrices &lt;../notebooks/class_2/week_3/00_welcome_to_week_3.html&gt;`_ (*see navigation bar on left*)
-**ND Arrays:**
-- `Arrays — From Welcome through Color Images as Arrays &lt;../notebooks/class_2/week_3/40_nd_arrays.html&gt;`_ (*see navigation bar on left*)</t>
   </si>
   <si>
     <t>- `Speed / Ease of Use Tradeoff &lt;../notebooks/class_2/week_4/10_speed_and_ease_of_use.html&gt;`_
@@ -262,23 +239,10 @@
 - `Pandas reshaping (with pics!) &lt;https://pandas.pydata.org/pandas-docs/stable/user_guide/reshaping.html&gt;`_</t>
   </si>
   <si>
-    <t>- `Understanding Performance &lt;../notebooks/class_2/week_4/10_speed_and_ease_of_use.html&gt;`_
-- `Improving Performance &lt;../notebooks/PDS_not_yet_in_coursera/30_big_data/50_performance_solutions.html&gt;`_
-- `Code Reviews &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/pr_review.html&gt;`_
-- Read all readings under the Statistical Modelling heading, starting with `Inference and Prediction &lt;../notebooks/class_5/week_3/20_inference_v_prediction.html&gt;`_ through `Beyond the Basic Model &lt;../notebooks/class_5/week_3/40_linear_regression_extensions&gt;`_</t>
-  </si>
-  <si>
-    <t>- `JVP Chapter 5 up to but not including Hyperparameters and Model Validation Section &lt;https://jakevdp.github.io/PythonDataScienceHandbook/#5.-Machine-Learning&gt;`_</t>
-  </si>
-  <si>
     <t>- ROUGH DRAFT OF OPIOID PROJECT DUE, extendable to Morning of Mon Nov 26 but feedback may be later</t>
   </si>
   <si>
     <t>- `Ex 1 &lt;../ids720_specific/exercises/Exercise_git.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Ex 1 &lt;../ids720_specific/exercises/Exercise_git_2.html&gt;`_
-- `Ex 2 &lt;../ids720_specific/exercises/Exercise_numpy_vectors.html&gt;`_</t>
   </si>
   <si>
     <t>- `Ex 1 &lt;../ids720_specific/exercises/Exercise_numpy_viewcopies.html&gt;`_
@@ -314,9 +278,6 @@
   </si>
   <si>
     <t>- `Link &lt;../ids720_specific/exercises/Exercise_statsmodels.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;../ids720_specific/exercises/Exercise_sklearn.html&gt;`_</t>
   </si>
   <si>
     <t>- Ideas Into Code</t>
@@ -359,17 +320,7 @@
 - `Ex 3 &lt;../ids720_specific/exercises/Exercise_jupytervscode.html&gt;`_</t>
   </si>
   <si>
-    <t>- Legos</t>
-  </si>
-  <si>
-    <t>- Using VS Code
-- Max, Triangle, and Retirement</t>
-  </si>
-  <si>
     <t>- Zendo</t>
-  </si>
-  <si>
-    <t>- Heart Rate Exercise</t>
   </si>
   <si>
     <t>- Point
@@ -424,6 +375,47 @@
   </si>
   <si>
     <t>- DSwithNSD1, Sets and Big-O Notation (and Dicts)</t>
+  </si>
+  <si>
+    <t>- Under the numpy heading, `read everything under Vectors EXCEPT Speed/Ease of Use Tradeoff and Vectorization &lt;../notebooks/class_2/week_2/10_why_numpy.html&gt;`_
+- Under the numpy heading, also read everything under `Subsetting Vectors &lt;../notebooks/class_2/week_2/10_why_numpy.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Ex 1 &lt;../ids720_specific/exercises/Exercise_numpy_vectors.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Matrices — From Welcome through Review of Matrices &lt;../notebooks/class_2/week_3/00_welcome_to_week_3.html&gt;`_ (*see navigation bar on left*)
+- `Arrays — From Welcome through Color Images as Arrays &lt;../notebooks/class_2/week_3/40_nd_arrays.html&gt;`_ (*see navigation bar on left*)</t>
+  </si>
+  <si>
+    <t>- `Views and Copies &lt;../notebooks/class_2/week_3/10_views_and_copies.html&gt;`_
+- `When Do I Get a View &lt;../notebooks/class_2/week_3/11_when_do_I_get_a_view.html&gt;`_
+- `Variables, Objects, and Numpy &lt;../notebooks/class_2/week_3/13_objects_and_variables.html&gt;`_
+- `Views and Copies Recap &lt;../notebooks/class_2/week_3/12_views_and_copies_recap.html&gt;`_
+**Additional Concepts**
+- `Numbers in Computers &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/ints_and_floats.html&gt;`_
+- `Writing Good Notebooks &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/writing_good_jupyter_notebooks.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- Git Day 2</t>
+  </si>
+  <si>
+    <t>- `Ex 2 &lt;../ids720_specific/exercises/Exercise_git_2.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- Heart Rate</t>
+  </si>
+  <si>
+    <t>- Read all readings under the Statistical Modelling heading, starting with `Inference and Prediction &lt;../notebooks/class_5/week_3/20_inference_v_prediction.html&gt;`_ through `Beyond the Basic Model &lt;../notebooks/class_5/week_3/40_linear_regression_extensions&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Legos &lt;../ids590_specific/exercises_590/10_lego_algorithm.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- Using VS Code
+- `Max &lt;../ids590_specific/exercises_590/20_max.html&gt;`_
+- Triangle
+- Retirement</t>
   </si>
 </sst>
 </file>
@@ -825,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -855,367 +847,365 @@
     </row>
     <row r="2" spans="1:4" ht="139" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>100</v>
-      </c>
       <c r="D8" s="11" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="43" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="57" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="B13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>67</v>
+        <v>47</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
+        <v>82</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>37</v>
-      </c>
       <c r="B23" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>72</v>
+        <v>4</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>73</v>
+        <v>37</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="11" t="s">
+      <c r="B26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="71" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="136" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update schedule for debugging
</commit_message>
<xml_diff>
--- a/ids590_specific/class_schedule_590_xlsx.xlsx
+++ b/ids590_specific/class_schedule_590_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids590_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3D2E1B-0475-7748-B3F9-B74CD5F3B120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DB1E94-76E4-8943-98D8-3B0389F45EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2540" yWindow="500" windowWidth="35860" windowHeight="19720" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -290,14 +290,6 @@
     <t>- Testing Your Code</t>
   </si>
   <si>
-    <t>- **SETUP 1:** `Installing Python and miniconda &lt;../notebooks/PDS_not_yet_in_coursera/00_setup_env/setup_python.html&gt;`_
-- **SETUP 2:** `Installing and Configuring VS Code &lt;../notebooks/PDS_not_yet_in_coursera/00_setup_env/setup_vscode.html&gt;`_
-- `chatGPT and You &lt;../notebooks/PDS_not_yet_in_coursera/99_advice/llms.html&gt;`_
-- `Read and sign syllabus, submit on gradescope &lt;https://github.com/nickeubank/practicaldatascience_book/raw/main/ids720_specific/syllabus/Syllabus_PracticalDataScience.pdf?download=&gt;`_
-- `Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
-- `Register for DataCamp &lt;https://www.datacamp.com/home&gt;`_</t>
-  </si>
-  <si>
     <t>- **SETUP 3:** `Setup Augmented Command Line &lt;../notebooks/PDS_not_yet_in_coursera/00_setup_env/setup_augmented_commandline.html&gt;`_
 - `Command Line Basics &lt;../notebooks/PDS_not_yet_in_coursera/10_commandline/commandline_part1.html&gt;`_
 - `Advanced Command Line &lt;../notebooks/PDS_not_yet_in_coursera/10_commandline/commandline_part2.html&gt;`_
@@ -340,20 +332,10 @@
     <t>- Start git?</t>
   </si>
   <si>
-    <t xml:space="preserve">- PPF1, Seven Steps for Algorithm Design
-- PPF1, Working an Example of the Seven Steps Process
-- PPF1, Data Types
-</t>
-  </si>
-  <si>
     <t>- DSwithNSD1, Basics of Object Oriented Programming</t>
   </si>
   <si>
     <t>- DSwithNSD1, Sets and Big-O Notation (and Dicts)</t>
-  </si>
-  <si>
-    <t>- Under the numpy heading, `read everything under Vectors EXCEPT Speed/Ease of Use Tradeoff and Vectorization &lt;../notebooks/class_2/week_2/10_why_numpy.html&gt;`_
-- Under the numpy heading, also read everything under `Subsetting Vectors &lt;../notebooks/class_2/week_2/10_why_numpy.html&gt;`_</t>
   </si>
   <si>
     <t>- `Ex 1 &lt;../ids720_specific/exercises/Exercise_numpy_vectors.html&gt;`_</t>
@@ -389,32 +371,51 @@
 - `Triangle &lt;../ids590_specific/exercises_590/30_triangle.html&gt;`_</t>
   </si>
   <si>
-    <t>- PPF2, Important Python Syntax
-- `Python v. R &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/python_v_r.html&gt;`_
+    <t>- `Debugging &lt;../ids720/exercises/Exercise_debugger.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- Buffer Day</t>
+  </si>
+  <si>
+    <t>Buffer day to allow extra time for any topics needing additional attention</t>
+  </si>
+  <si>
+    <t>- `List Max &lt;../ids590_specific/exercises_590/40_listmax.html&gt;`_
+- `HR Peak &lt;../ids590_specific/exercises_590/50_heartrate_peak.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- Under the numpy heading, `read everything under Vectors EXCEPT Speed/Ease of Use Tradeoff and Vectorization &lt;../notebooks/class_2/week_2/10_why_numpy.html&gt;`_
+- Under the numpy heading, also read everything under `Subsetting Vectors &lt;../notebooks/class_2/week_2/10_why_numpy.html&gt;`_
+- `Python v. R &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/python_v_r.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- **SETUP 1:** `Installing Python and miniconda &lt;../notebooks/PDS_not_yet_in_coursera/00_setup_env/setup_python.html&gt;`_
+- **SETUP 2:** `Installing and Configuring VS Code &lt;../notebooks/PDS_not_yet_in_coursera/00_setup_env/setup_vscode.html&gt;`_
+- `Read and sign syllabus, submit on gradescope &lt;https://github.com/nickeubank/practicaldatascience_book/raw/main/ids720_specific/syllabus/Syllabus_PracticalDataScience.pdf?download=&gt;`_
+- `Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
+- `Register for DataCamp &lt;https://www.datacamp.com/home&gt;`_</t>
+  </si>
+  <si>
+    <t>- PPF1, Seven Steps for Algorithm Design
+- PPF1, Working an Example of the Seven Steps Process
+- PPF1, **SKIP** Creating an Algorithm</t>
+  </si>
+  <si>
+    <t>- `chatGPT and You &lt;../notebooks/PDS_not_yet_in_coursera/99_advice/llms.html&gt;`_
+- PPF1, Data Types
+- PPF2, Important Python Syntax
 - PPF2, Translating an Algorithm Into Python
 - `f-strings &lt;../notebooks/other/fstrings.html&gt;`_</t>
   </si>
   <si>
-    <t>- `Debugging &lt;../ids720/exercises/Exercise_debugger.html&gt;`_</t>
-  </si>
-  <si>
     <t>- PPF3, Approaches to Testing
-- PPF3, Testing and Debugging
+- PPF4, Looking More into Lists. 
+    - Do NOT do List Max exercise or the Heart Rate programming assignments.</t>
+  </si>
+  <si>
+    <t>- Debugging (principles) &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/10_debugging_principles.html&gt;`_
+- Debugging (tools) &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/20_debugging_in_vscode.html&gt;`_
 - `What are Tracebacks? &lt;https://www.youtube.com/watch?v=JD8BrXXNtjA&gt;`_</t>
-  </si>
-  <si>
-    <t>- Buffer Day</t>
-  </si>
-  <si>
-    <t>Buffer day to allow extra time for any topics needing additional attention</t>
-  </si>
-  <si>
-    <t>- PPF4, Looking More into Lists. 
-    - Do NOT do List Max exercise or the Heart Rate programming assignments.</t>
-  </si>
-  <si>
-    <t>- `List Max &lt;../ids590_specific/exercises_590/40_listmax.html&gt;`_
-- `HR Peak &lt;../ids590_specific/exercises_590/50_heartrate_peak.html&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -818,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,7 +853,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="D2" s="7"/>
     </row>
@@ -864,13 +865,13 @@
         <v>69</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -878,13 +879,13 @@
         <v>68</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -892,24 +893,24 @@
         <v>70</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>99</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -917,10 +918,10 @@
         <v>22</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -928,13 +929,13 @@
         <v>23</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
@@ -942,10 +943,10 @@
         <v>24</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D9" s="11"/>
     </row>
@@ -954,16 +955,16 @@
         <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="43" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>26</v>
       </c>
@@ -971,10 +972,10 @@
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="170" x14ac:dyDescent="0.2">
@@ -985,7 +986,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>57</v>
@@ -999,7 +1000,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="57" x14ac:dyDescent="0.2">
@@ -1032,7 +1033,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -1040,7 +1041,7 @@
     </row>
     <row r="17" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>8</v>
@@ -1060,7 +1061,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>61</v>
@@ -1102,7 +1103,7 @@
         <v>9</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>67</v>
@@ -1161,7 +1162,7 @@
         <v>52</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="136" x14ac:dyDescent="0.2">
@@ -1186,10 +1187,10 @@
         <v>44</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update link to coursera
</commit_message>
<xml_diff>
--- a/ids590_specific/class_schedule_590_xlsx.xlsx
+++ b/ids590_specific/class_schedule_590_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids590_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62860339-F9C7-3941-B12C-C93B319487F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E6FF82-EFCD-544E-AE31-4B37A62E89C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -336,91 +336,91 @@
     <t>- Zendo if time</t>
   </si>
   <si>
+    <t>Tues, Aug 26</t>
+  </si>
+  <si>
+    <t>Thurs, Aug 28</t>
+  </si>
+  <si>
+    <t>Tues, Sep 2</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 4</t>
+  </si>
+  <si>
+    <t>Tues, Sep 9</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 11</t>
+  </si>
+  <si>
+    <t>Tues, Sep 16</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 18</t>
+  </si>
+  <si>
+    <t>Tues, Sep 23</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 25</t>
+  </si>
+  <si>
+    <t>Tues, Sep 30</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 2</t>
+  </si>
+  <si>
+    <t>Tues, Oct 7</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 9</t>
+  </si>
+  <si>
+    <t>Tues, Oct 14 (Break)</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 16 (Break)</t>
+  </si>
+  <si>
+    <t>Tues, Oct 21</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 23</t>
+  </si>
+  <si>
+    <t>Tues, Oct 28</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 30</t>
+  </si>
+  <si>
+    <t>Tues, Nov 4</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 6</t>
+  </si>
+  <si>
+    <t>Tues, Nov 11</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 13</t>
+  </si>
+  <si>
+    <t>Tues, Nov 18</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 220</t>
+  </si>
+  <si>
     <t>- **SETUP 1:** `Installing Python and miniconda &lt;../notebooks/PDS_not_yet_in_coursera/00_setup_env/setup_python.html&gt;`_
 - **SETUP 2:** `Installing and Configuring VS Code &lt;../notebooks/PDS_not_yet_in_coursera/00_setup_env/setup_vscode.html&gt;`_
 - `Read and sign syllabus, submit on gradescope &lt;https://github.com/nickeubank/practicaldatascience_book/blob/main/ids590_specific/syllabus_590/Syllabus_IDS590.pdf?download=&gt;`_
 - `Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
 - `Join Slack Group &lt;https://join.slack.com/t/pds1-2025/shared_invite/zt-3bzo97p3a-Q~Om4Ft2ABhuA0n0Gz7Pjw&gt;`_
 - `Register for DataCamp (duke.edu address required) &lt;https://www.datacamp.com/groups/shared_links/8bb72514ddc2ab2831e57a4622f46f79a3f94bc8dda25587c0e12199d6ff0a59&gt;`_
-- `Join Coursera IDS 590 Session of Python Programming Fundamentals &lt;https://coursera.org/groups/python-programming-fundamentals-ec2do&gt;`_</t>
-  </si>
-  <si>
-    <t>Tues, Aug 26</t>
-  </si>
-  <si>
-    <t>Thurs, Aug 28</t>
-  </si>
-  <si>
-    <t>Tues, Sep 2</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 4</t>
-  </si>
-  <si>
-    <t>Tues, Sep 9</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 11</t>
-  </si>
-  <si>
-    <t>Tues, Sep 16</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 18</t>
-  </si>
-  <si>
-    <t>Tues, Sep 23</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 25</t>
-  </si>
-  <si>
-    <t>Tues, Sep 30</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 2</t>
-  </si>
-  <si>
-    <t>Tues, Oct 7</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 9</t>
-  </si>
-  <si>
-    <t>Tues, Oct 14 (Break)</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 16 (Break)</t>
-  </si>
-  <si>
-    <t>Tues, Oct 21</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 23</t>
-  </si>
-  <si>
-    <t>Tues, Oct 28</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 30</t>
-  </si>
-  <si>
-    <t>Tues, Nov 4</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 6</t>
-  </si>
-  <si>
-    <t>Tues, Nov 11</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 13</t>
-  </si>
-  <si>
-    <t>Tues, Nov 18</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 220</t>
+- `Join Coursera IDS 590 Session of Python Programming Fundamentals &lt;https://coursera.org/groups/python-programming-fundamentals-ec2do/invitation&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,19 +852,19 @@
     </row>
     <row r="2" spans="1:4" ht="139" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>45</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="4" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>44</v>
@@ -892,7 +892,7 @@
     </row>
     <row r="5" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>46</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>49</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>66</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>52</v>
@@ -948,7 +948,7 @@
     </row>
     <row r="9" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>52</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="10" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>48</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>5</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="12" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>5</v>
@@ -1002,7 +1002,7 @@
     </row>
     <row r="13" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>12</v>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="14" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>6</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="15" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>7</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="17" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>8</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="18" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>10</v>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="19" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>16</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="20" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>16</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="21" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>9</v>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="22" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>13</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="23" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>4</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="24" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>15</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="25" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>19</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="26" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>20</v>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
update with text for wordcount
</commit_message>
<xml_diff>
--- a/ids590_specific/class_schedule_590_xlsx.xlsx
+++ b/ids590_specific/class_schedule_590_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids590_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EF8A8C-877F-DA44-AA6D-B19C6EBF57B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FB31BB-EFF1-A847-AD63-6253D5D67983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-220" yWindow="1340" windowWidth="30240" windowHeight="17500" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="0" yWindow="1340" windowWidth="36260" windowHeight="20160" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule_590" sheetId="1" r:id="rId1"/>
@@ -234,10 +234,6 @@
 - `Ex 3 &lt;../ids720_specific/exercises/Exercise_jupytervscode.html&gt;`_</t>
   </si>
   <si>
-    <t>- Point
-- Circle</t>
-  </si>
-  <si>
     <t>- Object Oriented Programming</t>
   </si>
   <si>
@@ -417,6 +413,10 @@
   </si>
   <si>
     <t>- `Func Diagrams &lt;../ids590_specific/exercises_590/Exercise_function_stack_diagrams.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Point &lt;../ids590_specific/exercises_590/60_point.html&gt;`_
+- Circle</t>
   </si>
 </sst>
 </file>
@@ -824,7 +824,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -851,126 +851,126 @@
     </row>
     <row r="2" spans="1:4" ht="139" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>43</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>46</v>
@@ -984,27 +984,27 @@
     </row>
     <row r="12" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>31</v>
@@ -1012,18 +1012,18 @@
     </row>
     <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>6</v>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="16" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>7</v>
@@ -1051,7 +1051,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="18" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>8</v>
@@ -1073,13 +1073,13 @@
     </row>
     <row r="19" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>35</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="20" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>16</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="21" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>16</v>
@@ -1115,13 +1115,13 @@
     </row>
     <row r="22" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>41</v>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>13</v>
@@ -1143,7 +1143,7 @@
     </row>
     <row r="24" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>4</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="25" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>15</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="26" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>18</v>
@@ -1180,12 +1180,12 @@
         <v>27</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>19</v>
@@ -1202,7 +1202,7 @@
         <v>17</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" s="11"/>
     </row>

</xml_diff>

<commit_message>
add one more day for command line
</commit_message>
<xml_diff>
--- a/ids590_specific/class_schedule_590_xlsx.xlsx
+++ b/ids590_specific/class_schedule_590_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids590_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE3A559-6B2F-CF46-827C-087A18DBDB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819122E7-7985-8A4D-9779-08C9B66E7262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="99">
   <si>
     <t>Topic</t>
   </si>
@@ -107,14 +107,6 @@
 - `Matplotlib Vocabulary &lt;../notebooks/class_5/week_1/1.2.2_ten_figure_pieces.html&gt;`_
 - `Explicit v Implict &lt;../notebooks/class_5/week_1/1.4.5_explicit_vs_implicit_syntax.html&gt;`_
 - `Saving Plots &lt;../notebooks/class_5/week_1/1.4.4_saving_to_file.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Plotting in Python through seaborn and Grammer of Graphics &lt;../notebooks/class_5/week_1/2.3.1_plotting_with_seaborn.html&gt;`_
-- `seaborn recipes &lt;../notebooks/class_5/week_1/2.3.2_seaborn_recipes.html&gt;`_
-- `Customizing matplotlib &lt;../notebooks/class_5/week_1/2.1.2_customizing_plot_styles.html&gt;`_
-- `Making Pretty Plots 1 &lt;../notebooks/class_5/week_1/2.2.1_making_plots_pretty_1.html&gt;`_
-- `Making Pretty Plots 2 &lt;../notebooks/class_5/week_1/2.2.2_making_plots_pretty_2.html&gt;`_
-- `Pandas Plotting &lt;../notebooks/class_5/week_1/1.6.1_plotting_with_pandas.html&gt;`_</t>
   </si>
   <si>
     <t>- `Combining, Grouping and Querying &lt;../notebooks/class_3/week_4/00_intro_to_querying_data.html&gt;`_
@@ -147,9 +139,6 @@
   </si>
   <si>
     <t>- `Link &lt;../ids720_specific/exercises/Exercise_plotting_part1.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;../ids720_specific/exercises/Exercise_plotting_part2.html&gt;`_</t>
   </si>
   <si>
     <t>- `Link &lt;../ids720_specific/exercises/Exercise_merging.html&gt;`_</t>
@@ -400,6 +389,9 @@
   <si>
     <t>- Data Cleaning  from `Identifying Problems &lt;../notebooks/class_3/week_3/20_cleaning_identifying.html&gt;`_ through `Cleaning Data Types &lt;../notebooks/class_3/week_3/33_cleaning_datatypes.html&gt;`_
 - `Datacamp Class "Regular Expressions for Pattern Matching," Chapter 3 (Introduction to regular expressions) &lt;https://campus.datacamp.com/courses/regular-expressions-in-python/basic-concepts-of-string-manipulation?ex=1&gt;`_</t>
+  </si>
+  <si>
+    <t>More command line</t>
   </si>
 </sst>
 </file>
@@ -806,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,349 +826,343 @@
     </row>
     <row r="2" spans="1:4" ht="139" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" t="s">
         <v>89</v>
-      </c>
-      <c r="D9" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="57" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="170" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
-        <v>65</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>44</v>
+      <c r="C15" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="D19" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>98</v>
+        <v>69</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>45</v>
+        <v>72</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="71" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
+    </row>
+    <row r="27" spans="1:4" ht="71" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="90" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="D27" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1184,7 +1170,7 @@
         <v>15</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C28" s="11"/>
     </row>

</xml_diff>

<commit_message>
build with lowercase exercises
</commit_message>
<xml_diff>
--- a/ids590_specific/class_schedule_590_xlsx.xlsx
+++ b/ids590_specific/class_schedule_590_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids590_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D48715-C3AC-6944-98F4-EF1083745790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4631683-C4C0-3B45-B733-D1AA33CF1F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="500" windowWidth="30240" windowHeight="17680" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -121,35 +121,6 @@
 - `Groupby &lt;../notebooks/class_3/week_4/20_grouping.html&gt;`_</t>
   </si>
   <si>
-    <t>- `Ex 1 &lt;../ids720_specific/exercises/Exercise_numpy_viewcopies.html&gt;`_
-- (Finish other numpy)</t>
-  </si>
-  <si>
-    <t>- `Link &lt;../ids720_specific/exercises/Exercise_series.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;../ids720_specific/exercises/Exercise_dataframes.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link 1 &lt;../ids720_specific/exercises/Exercise_indices.html&gt;`_
-- `Link 2 &lt;../ids720_specific/exercises/Exercise_missing.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;../ids720_specific/exercises/Exercise_cleaning.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;../ids720_specific/exercises/Exercise_plotting_part1.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;../ids720_specific/exercises/Exercise_merging.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;../ids720_specific/exercises/Exercise_groupby.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;../ids720_specific/exercises/Exercise_statsmodels.html&gt;`_</t>
-  </si>
-  <si>
     <t>- Ideas Into Code</t>
   </si>
   <si>
@@ -177,18 +148,10 @@
     <t>- Lists In Depth</t>
   </si>
   <si>
-    <t>- `Ex 1 &lt;../ids720_specific/exercises/Exercise_CommandLine_1_Basics.html&gt;`_
-- `Ex 2 &lt;../ids720_specific/exercises/Exercise_CommandLine_2_Advanced.html&gt;`_
-- `Ex 3 &lt;../ids720_specific/exercises/Exercise_jupytervscode.html&gt;`_</t>
-  </si>
-  <si>
     <t>- Object Oriented Programming</t>
   </si>
   <si>
     <t>- DSwithNSD1, Sets and Big-O Notation (and Dicts)</t>
-  </si>
-  <si>
-    <t>- `Ex 1 &lt;../ids720_specific/exercises/Exercise_numpy_vectors.html&gt;`_</t>
   </si>
   <si>
     <t>- `Matrices — From Welcome through Review of Matrices &lt;../notebooks/class_2/week_3/00_welcome_to_week_3.html&gt;`_ (*see navigation bar on left*)
@@ -332,16 +295,10 @@
 - DSwithNSD1, Basics of Object Oriented Programming</t>
   </si>
   <si>
-    <t>- `Debugging &lt;../ids590_specific/exercises_590/Exercise_debugger590.html&gt;`_</t>
-  </si>
-  <si>
     <t>- `Blackjack &lt;../ids590_specific/exercises_590/35_blackjack.html&gt;`_</t>
   </si>
   <si>
     <t>- List Practice</t>
-  </si>
-  <si>
-    <t>- `Func Diagrams &lt;../ids590_specific/exercises_590/Exercise_function_stack_diagrams.html&gt;`_</t>
   </si>
   <si>
     <t>- `Debugging (principles) &lt;../notebooks/PDS_not_yet_in_coursera/20_programming_concepts/10_debugging_principles.html&gt;`_
@@ -380,9 +337,6 @@
     <t>- `JVP Chapter 5 up to but not including Hyperparameters and Model Validation Section &lt;https://jakevdp.github.io/PythonDataScienceHandbook/#5.-Machine-Learning&gt;`_</t>
   </si>
   <si>
-    <t>- `Link &lt;exercises/Exercise_sklearn.html&gt;`_</t>
-  </si>
-  <si>
     <t>- Pandas: Cleaning
 - Regex</t>
   </si>
@@ -395,6 +349,52 @@
   </si>
   <si>
     <t>- `Ex 1 &lt;../ids590_specific/exercises_590/90_remote_sensing.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Func Diagrams &lt;../ids590_specific/exercises_590/exercise_function_stack_diagrams.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Debugging &lt;../ids590_specific/exercises_590/exercise_debugger590.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Ex 1 &lt;../ids720_specific/exercises/exercise_CommandLine_1_Basics.html&gt;`_
+- `Ex 2 &lt;../ids720_specific/exercises/exercise_CommandLine_2_Advanced.html&gt;`_
+- `Ex 3 &lt;../ids720_specific/exercises/exercise_jupytervscode.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Ex 1 &lt;../ids720_specific/exercises/exercise_numpy_vectors.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Ex 1 &lt;../ids720_specific/exercises/exercise_numpy_viewcopies.html&gt;`_
+- (Finish other numpy)</t>
+  </si>
+  <si>
+    <t>- `Link &lt;../ids720_specific/exercises/exercise_series.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link &lt;../ids720_specific/exercises/exercise_dataframes.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link 1 &lt;../ids720_specific/exercises/exercise_indices.html&gt;`_
+- `Link 2 &lt;../ids720_specific/exercises/exercise_missing.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link &lt;../ids720_specific/exercises/exercise_cleaning.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link &lt;../ids720_specific/exercises/exercise_groupby.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link &lt;../ids720_specific/exercises/exercise_merging.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link &lt;../ids720_specific/exercises/exercise_statsmodels.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link &lt;exercises/exercise_sklearn.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link &lt;../ids720_specific/exercises/exercise_plotting_part1.html&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -802,7 +802,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -829,209 +829,209 @@
     </row>
     <row r="2" spans="1:4" ht="139" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C5" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="18" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>5</v>
@@ -1048,12 +1048,12 @@
         <v>16</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>6</v>
@@ -1062,12 +1062,12 @@
         <v>17</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>7</v>
@@ -1076,26 +1076,26 @@
         <v>18</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>11</v>
@@ -1104,12 +1104,12 @@
         <v>21</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>13</v>
@@ -1118,40 +1118,40 @@
         <v>20</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="71" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>14</v>
@@ -1160,15 +1160,15 @@
         <v>19</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1176,7 +1176,7 @@
         <v>15</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C28" s="11"/>
     </row>

</xml_diff>

<commit_message>
update with rough draft
</commit_message>
<xml_diff>
--- a/ids590_specific/class_schedule_590_xlsx.xlsx
+++ b/ids590_specific/class_schedule_590_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids590_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC24E518-E906-5B4C-A8A6-BC4EAE3C1D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A36699-B977-B84C-A5C1-02A1EBB7C373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
   <si>
     <t>Topic</t>
   </si>
@@ -331,12 +331,6 @@
     <t>- More OOP</t>
   </si>
   <si>
-    <t>- Machine Learning with sckikit-learn</t>
-  </si>
-  <si>
-    <t>- `JVP Chapter 5 up to but not including Hyperparameters and Model Validation Section &lt;https://jakevdp.github.io/PythonDataScienceHandbook/#5.-Machine-Learning&gt;`_</t>
-  </si>
-  <si>
     <t>- Pandas: Cleaning
 - Regex</t>
   </si>
@@ -382,16 +376,10 @@
     <t>- `Link &lt;../ids720_specific/exercises/exercise_cleaning.html&gt;`_</t>
   </si>
   <si>
-    <t>- `Link &lt;../ids720_specific/exercises/exercise_groupby.html&gt;`_</t>
-  </si>
-  <si>
     <t>- `Link &lt;../ids720_specific/exercises/exercise_merging.html&gt;`_</t>
   </si>
   <si>
     <t>- `Link &lt;../ids720_specific/exercises/exercise_statsmodels.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Link &lt;exercises/exercise_sklearn.html&gt;`_</t>
   </si>
   <si>
     <t>- `Link &lt;../ids720_specific/exercises/exercise_plotting_part1.html&gt;`_</t>
@@ -406,6 +394,16 @@
   </si>
   <si>
     <t>- `Link &lt;exercises/exercise_plotting_part2.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link &lt;../ids720_specific/exercises/exercise_groupby.html&gt;`_
+- `Opioids Project &lt;https://github.com/nickeubank/practicaldatascience_book/blob/main/ids590_specific/opioids_590/PDS590_ProjectSummary.pdf&gt;`_</t>
+  </si>
+  <si>
+    <t>- Discuss Opioids Project</t>
+  </si>
+  <si>
+    <t>- Opioids Working Session</t>
   </si>
 </sst>
 </file>
@@ -813,7 +811,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -889,7 +887,7 @@
         <v>73</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -903,7 +901,7 @@
         <v>71</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -995,7 +993,7 @@
         <v>25</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="57" x14ac:dyDescent="0.2">
@@ -1009,7 +1007,7 @@
         <v>36</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="170" x14ac:dyDescent="0.2">
@@ -1023,7 +1021,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1045,7 +1043,7 @@
         <v>30</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="57" x14ac:dyDescent="0.2">
@@ -1059,7 +1057,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -1073,7 +1071,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -1087,7 +1085,7 @@
         <v>18</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
@@ -1095,13 +1093,13 @@
         <v>58</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
@@ -1114,8 +1112,8 @@
       <c r="C22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>95</v>
+      <c r="D22" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="102" x14ac:dyDescent="0.2">
@@ -1129,7 +1127,7 @@
         <v>20</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
@@ -1143,7 +1141,7 @@
         <v>32</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
@@ -1157,7 +1155,7 @@
         <v>19</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="90" x14ac:dyDescent="0.2">
@@ -1165,27 +1163,24 @@
         <v>63</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>65</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update final project due-date
</commit_message>
<xml_diff>
--- a/ids590_specific/class_schedule_590_xlsx.xlsx
+++ b/ids590_specific/class_schedule_590_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids590_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F87E18-1914-B749-B9B6-8CD252990BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2927DDA8-FAB9-6A47-8C5B-E393BA2D5B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t>- Plotting</t>
   </si>
   <si>
-    <t>Wed Dec 12</t>
-  </si>
-  <si>
     <t>- `Speed / Ease of Use Tradeoff &lt;../notebooks/class_2/week_4/10_speed_and_ease_of_use.html&gt;`_
 - `Vectorization &lt;../notebooks/class_2/week_4/11_vectorization.html&gt;`_
 - Under Pandas, Read from `From Working with Tabular Data &lt;../notebooks/class_3/week_2/00_intro_to_pandas.html&gt;`_ through `Subsetting and Indexing with Single Square Brackets &lt;../notebooks/class_3/week_2/16_indexing_with_brackets.html&gt;`_</t>
@@ -100,13 +97,6 @@
 - `Views and Copies in Pandas &lt;../notebooks/class_3/week_3/10_views_and_copies_numpy_review.html&gt;`_ through `the View/Copy Headache without CoW &lt;../notebooks/class_3/week_3/17_views_and_copies_in_pandas_wo_CoW.html&gt;`_
 - Reading and Writing Data: `Read from Ways To Store and Read Data &lt;../notebooks/class_3/week_3/00_plaintext_files.html&gt;`_ through ways to `Store and Read Binary Data &lt;../notebooks/class_3/week_3/05_binary_files.html&gt;`_
 - `Missing Data &lt;../notebooks/class_3/week_3/35_cleaning_missing_data.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Plotting Principles &lt;../notebooks/class_5/week_1/1.1.2_effective_plotting_practices.html&gt;`_
-- `Matplotlib Basics &lt;../notebooks/class_5/week_1/1.2.1_basic_plotting_with_matplotlib.html&gt;`_
-- `Matplotlib Vocabulary &lt;../notebooks/class_5/week_1/1.2.2_ten_figure_pieces.html&gt;`_
-- `Explicit v Implict &lt;../notebooks/class_5/week_1/1.4.5_explicit_vs_implicit_syntax.html&gt;`_
-- `Saving Plots &lt;../notebooks/class_5/week_1/1.4.4_saving_to_file.html&gt;`_</t>
   </si>
   <si>
     <t>- `Combining, Grouping and Querying &lt;../notebooks/class_3/week_4/00_intro_to_querying_data.html&gt;`_
@@ -401,6 +391,17 @@
   </si>
   <si>
     <t>- Opioids Working Session</t>
+  </si>
+  <si>
+    <t>- `Plotting Principles &lt;../notebooks/class_5/week_1/1.1.2_effective_plotting_practices.html&gt;`_
+- `Matplotlib Basics &lt;../notebooks/class_5/week_1/1.2.1_basic_plotting_with_matplotlib.html&gt;`_
+- `Matplotlib Vocabulary &lt;../notebooks/class_5/week_1/1.2.2_ten_figure_pieces.html&gt;`_
+- `Explicit v Implict &lt;../notebooks/class_5/week_1/1.4.5_explicit_vs_implicit_syntax.html&gt;`_
+- `Saving Plots &lt;../notebooks/class_5/week_1/1.4.4_saving_to_file.html&gt;`_
+- `Using LLMs Well &lt;../notebooks/PDS_not_yet_in_coursera/99_advice/using_llms_well.html&gt;`_</t>
+  </si>
+  <si>
+    <t>Wed Dec 10</t>
   </si>
 </sst>
 </file>
@@ -807,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -835,195 +836,195 @@
     </row>
     <row r="2" spans="1:4" ht="139" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>72</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
         <v>74</v>
-      </c>
-      <c r="D9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
@@ -1031,158 +1032,158 @@
     </row>
     <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C28" s="11"/>
     </row>

</xml_diff>

<commit_message>
add plotting to matplotlib
</commit_message>
<xml_diff>
--- a/ids590_specific/class_schedule_590_xlsx.xlsx
+++ b/ids590_specific/class_schedule_590_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids590_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5044866-F837-214E-8BBF-222AA38053A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0E5E27-F83D-0B4B-A8AF-974641685599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="3240" windowWidth="30240" windowHeight="17680" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="4680" yWindow="2300" windowWidth="30240" windowHeight="17680" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule_590" sheetId="1" r:id="rId1"/>
@@ -375,14 +375,6 @@
     <t>- `Link &lt;../ids720_specific/exercises/exercise_plotting_part1.html&gt;`_</t>
   </si>
   <si>
-    <t>- `Plotting in Python through seaborn and Grammer of Graphics &lt;../notebooks/class_5/week_1/2.3.1_plotting_with_seaborn.html&gt;`_
-- `seaborn recipes &lt;../notebooks/class_5/week_1/2.3.2_seaborn_recipes.html&gt;`_
-- `Customizing matplotlib &lt;../notebooks/class_5/week_1/2.1.2_customizing_plot_styles.html&gt;`_
-- `Making Pretty Plots 1 &lt;../notebooks/class_5/week_1/2.2.1_making_plots_pretty_1.html&gt;`_
-- `Making Pretty Plots 2 &lt;../notebooks/class_5/week_1/2.2.2_making_plots_pretty_2.html&gt;`_
-- `Pandas Plotting &lt;../notebooks/class_5/week_1/1.6.1_plotting_with_pandas.html&gt;`_</t>
-  </si>
-  <si>
     <t>- `Link &lt;exercises/exercise_plotting_part2.html&gt;`_</t>
   </si>
   <si>
@@ -402,6 +394,15 @@
   </si>
   <si>
     <t>- Groupby Continued</t>
+  </si>
+  <si>
+    <t>- `Plotting in Python through seaborn and Grammer of Graphics &lt;../notebooks/class_5/week_1/2.3.1_plotting_with_seaborn.html&gt;`_
+- `seaborn recipes &lt;../notebooks/class_5/week_1/2.3.2_seaborn_recipes.html&gt;`_
+- `From seaborn to matplotlib &lt;../notebooks/class_5/week_1/2.3.3_from_seaborn_to_matplotlib.html&gt;`_
+- `Customizing matplotlib &lt;../notebooks/class_5/week_1/2.1.2_customizing_plot_styles.html&gt;`_
+- `Making Pretty Plots 1 &lt;../notebooks/class_5/week_1/2.2.1_making_plots_pretty_1.html&gt;`_
+- `Making Pretty Plots 2 &lt;../notebooks/class_5/week_1/2.2.2_making_plots_pretty_2.html&gt;`_
+- `Pandas Plotting &lt;../notebooks/class_5/week_1/1.6.1_plotting_with_pandas.html&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -809,7 +810,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1111,7 +1112,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1119,10 +1120,10 @@
         <v>58</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
@@ -1147,13 +1148,13 @@
         <v>14</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="90" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>61</v>
       </c>
@@ -1161,10 +1162,10 @@
         <v>80</v>
       </c>
       <c r="C26" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="43" x14ac:dyDescent="0.2">
@@ -1183,7 +1184,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>64</v>

</xml_diff>